<commit_message>
Code Cleanup & Added TaskChain
+ Code cleanup (Bad comments / Class names / Duplications)
+ Auto WhatsApp disconnecter added. (Socket connection only on when required to send message)
+ Made TaskChain for query messages until connection and Cache register.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A850066-B25F-4388-9257-464E287D7CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63683F26-75F2-4B31-BA0C-45B5E1C04AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -587,7 +587,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1">
-        <v>44451.754513888889</v>
+        <v>44454.076388888891</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
BugFix & Removed Feature & Updated Roadmap
+ Added QRAuthorize.java
+ Added JFrame QRCode printer for initial run.
+ Removed TaskChain reason of new WhatsApp upcoming update.
+ Added Command Feature to TODO List.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63683F26-75F2-4B31-BA0C-45B5E1C04AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5208F960-034B-4557-8B33-1D46197379FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -587,7 +587,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1">
-        <v>44454.076388888891</v>
+        <v>44455.027777777781</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>

</xml_diff>